<commit_message>
Populando a base de dados com dataset do DATASUS
</commit_message>
<xml_diff>
--- a/3_Hospital/database/Pentaho/especialidades.xlsx
+++ b/3_Hospital/database/Pentaho/especialidades.xlsx
@@ -24,16 +24,16 @@
     <t>Descricao</t>
   </si>
   <si>
-    <t>Nova Especialidade</t>
-  </si>
-  <si>
     <t>Cardilogia</t>
   </si>
   <si>
     <t>Pediatria</t>
   </si>
   <si>
-    <t>...</t>
+    <t>Clínico</t>
+  </si>
+  <si>
+    <t>Infectologia</t>
   </si>
 </sst>
 </file>
@@ -368,12 +368,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -389,7 +389,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -397,7 +397,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -405,7 +405,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">

</xml_diff>